<commit_message>
Decreased number of classes
</commit_message>
<xml_diff>
--- a/Model Tagging/data/Data Analysis.xlsx
+++ b/Model Tagging/data/Data Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MLeno\Documents\Code\machining-feature-recognition\Model Tagging\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\Code\machining-feature-recognition\Model Tagging\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB28551-97AB-4943-814B-117F95187CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DE3A87-269B-41E4-A288-DFB9CAF1F8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FD6EA7AA-67A1-4436-9947-EE9481BE3C2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FD6EA7AA-67A1-4436-9947-EE9481BE3C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
   <si>
     <t>Class</t>
   </si>
@@ -123,37 +123,190 @@
 (one-of-n)</t>
   </si>
   <si>
-    <t>Adjacent faces in an outer loop (1/11)</t>
+    <t>Adjacent unknown convexity  unknown geometry faces in an outer loop</t>
   </si>
   <si>
-    <t>Adjacent faces in an outer loop (2/11)</t>
+    <t>Adjacent unknown convexity bezier surface faces in an outer loop</t>
   </si>
   <si>
-    <t>Adjacent faces in an outer loop (3/11)</t>
+    <t>Adjacent unknown convexity bspline surface faces in an outer loop</t>
   </si>
   <si>
-    <t>Adjacent faces in an outer loop (4/11)</t>
+    <t>Adjacent unknown convexity rectangular trimmed  faces in an outer loop</t>
   </si>
   <si>
-    <t>Adjacent faces in an outer loop (5/11)</t>
+    <t>Adjacent unknown convexity conical faces in an outer loop</t>
   </si>
   <si>
-    <t>Adjacent faces in an outer loop (6/11)</t>
+    <t>Adjacent unknown convexity cylindrical faces in an outer loop</t>
   </si>
   <si>
-    <t>Adjacent faces in an outer loop (7/11)</t>
+    <t>Adjacent unknown convexity planar faces in an outer loop</t>
   </si>
   <si>
-    <t>Adjacent faces in an outer loop (8/11)</t>
+    <t>Adjacent unknown convexity spherical  faces in an outer loop</t>
   </si>
   <si>
-    <t>Adjacent faces in an outer loop (9/11)</t>
+    <t>Adjacent unknown convexity toroidal faces in an outer loop</t>
   </si>
   <si>
-    <t>Adjacent faces in an outer loop (10/11)</t>
+    <t>Adjacent unknown convexity linear extrusion surface faces in an outer loop</t>
   </si>
   <si>
-    <t>Adjacent faces in an outer loop (11/11)</t>
+    <t>Adjacent unknown convexity revolved surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent concave unknown geometry faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent concave bezier surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent concave bspline surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent concave rectangular trimmed  faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent concave conical faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent concave cylindrical faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent concave planar faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent concave spherical  faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent concave toroidal faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent concave linear extrusion surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent concave revolved surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent convex unknown geometry faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent convex bezier surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent convex bspline surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent convex rectangular trimmed  faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent convex conical faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent convex cylindrical faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent convex planar faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent convex spherical  faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent convex toroidal faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent convex linear extrusion surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent convex revolved surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent non-tangent  unknown geometry faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent non-tangent  bezier surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent non-tangent  bspline surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent non-tangent  rectangular trimmed  faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent non-tangent  conical faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent non-tangent  cylindrical faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent non-tangent  planar faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent non-tangent  spherical  faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent non-tangent  toroidal faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent non-tangent  linear extrusion surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent non-tangent  revolved surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent perpendicular  unknown geometry faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent perpendicular  bezier surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent perpendicular  bspline surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent perpendicular  rectangular trimmed  faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent perpendicular  conical faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent perpendicular  cylindrical faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent perpendicular  planar faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent perpendicular  spherical  faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent perpendicular  toroidal faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent perpendicular  linear extrusion surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Adjacent perpendicular  revolved surface faces in an outer loop</t>
+  </si>
+  <si>
+    <t>Contain concave inner loop that is not centered on face?</t>
+  </si>
+  <si>
+    <t>Contain convex inner loop that is centered on face?</t>
+  </si>
+  <si>
+    <t>None Features</t>
+  </si>
+  <si>
+    <t>Hole</t>
+  </si>
+  <si>
+    <t>Hole Feature</t>
+  </si>
+  <si>
+    <t>Pocket/Island/Slot</t>
+  </si>
+  <si>
+    <t>Fillet/Chamfer</t>
   </si>
 </sst>
 </file>
@@ -222,11 +375,6 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="1">
-          <cell r="A1">
-            <v>10</v>
-          </cell>
-        </row>
         <row r="2">
           <cell r="A2">
             <v>10</v>
@@ -244,7 +392,7 @@
         </row>
         <row r="5">
           <cell r="A5">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="6">
@@ -284,7 +432,7 @@
         </row>
         <row r="13">
           <cell r="A13">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="14">
@@ -314,7 +462,7 @@
         </row>
         <row r="19">
           <cell r="A19">
-            <v>4</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="20">
@@ -334,7 +482,7 @@
         </row>
         <row r="23">
           <cell r="A23">
-            <v>1</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="24">
@@ -384,12 +532,12 @@
         </row>
         <row r="33">
           <cell r="A33">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="34">
           <cell r="A34">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="35">
@@ -404,17 +552,17 @@
         </row>
         <row r="37">
           <cell r="A37">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="38">
           <cell r="A38">
-            <v>2</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="39">
           <cell r="A39">
-            <v>10</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="40">
@@ -429,7 +577,7 @@
         </row>
         <row r="42">
           <cell r="A42">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="43">
@@ -459,12 +607,12 @@
         </row>
         <row r="48">
           <cell r="A48">
-            <v>2</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="49">
           <cell r="A49">
-            <v>10</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="50">
@@ -514,7 +662,7 @@
         </row>
         <row r="59">
           <cell r="A59">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="60">
@@ -549,7 +697,7 @@
         </row>
         <row r="66">
           <cell r="A66">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="67">
@@ -574,7 +722,7 @@
         </row>
         <row r="71">
           <cell r="A71">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="72">
@@ -584,17 +732,17 @@
         </row>
         <row r="73">
           <cell r="A73">
-            <v>0</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="74">
           <cell r="A74">
-            <v>13</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="75">
           <cell r="A75">
-            <v>1</v>
+            <v>13</v>
           </cell>
         </row>
         <row r="76">
@@ -609,12 +757,12 @@
         </row>
         <row r="78">
           <cell r="A78">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="79">
           <cell r="A79">
-            <v>12</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="80">
@@ -659,27 +807,27 @@
         </row>
         <row r="88">
           <cell r="A88">
-            <v>0</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="89">
           <cell r="A89">
-            <v>12</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="90">
           <cell r="A90">
-            <v>0</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="91">
           <cell r="A91">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="92">
           <cell r="A92">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="93">
@@ -689,7 +837,7 @@
         </row>
         <row r="94">
           <cell r="A94">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="95">
@@ -709,7 +857,7 @@
         </row>
         <row r="98">
           <cell r="A98">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="99">
@@ -724,7 +872,7 @@
         </row>
         <row r="101">
           <cell r="A101">
-            <v>0</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="102">
@@ -739,7 +887,7 @@
         </row>
         <row r="104">
           <cell r="A104">
-            <v>12</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="105">
@@ -759,17 +907,17 @@
         </row>
         <row r="108">
           <cell r="A108">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="109">
           <cell r="A109">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="110">
           <cell r="A110">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="111">
@@ -779,12 +927,12 @@
         </row>
         <row r="112">
           <cell r="A112">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="113">
           <cell r="A113">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="114">
@@ -799,32 +947,32 @@
         </row>
         <row r="116">
           <cell r="A116">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="117">
           <cell r="A117">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="118">
           <cell r="A118">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="119">
           <cell r="A119">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="120">
           <cell r="A120">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="121">
           <cell r="A121">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="122">
@@ -834,37 +982,37 @@
         </row>
         <row r="123">
           <cell r="A123">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="124">
           <cell r="A124">
-            <v>14</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="125">
           <cell r="A125">
-            <v>1</v>
+            <v>14</v>
           </cell>
         </row>
         <row r="126">
           <cell r="A126">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="127">
           <cell r="A127">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="128">
           <cell r="A128">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="129">
           <cell r="A129">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="130">
@@ -879,12 +1027,12 @@
         </row>
         <row r="132">
           <cell r="A132">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="133">
           <cell r="A133">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="134">
@@ -894,12 +1042,12 @@
         </row>
         <row r="135">
           <cell r="A135">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="136">
           <cell r="A136">
-            <v>5</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="137">
@@ -909,7 +1057,7 @@
         </row>
         <row r="138">
           <cell r="A138">
-            <v>1</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="139">
@@ -959,7 +1107,7 @@
         </row>
         <row r="148">
           <cell r="A148">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="149">
@@ -969,7 +1117,7 @@
         </row>
         <row r="150">
           <cell r="A150">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="151">
@@ -979,7 +1127,7 @@
         </row>
         <row r="152">
           <cell r="A152">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="153">
@@ -999,7 +1147,7 @@
         </row>
         <row r="156">
           <cell r="A156">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="157">
@@ -1024,17 +1172,17 @@
         </row>
         <row r="161">
           <cell r="A161">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="162">
           <cell r="A162">
-            <v>10</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="163">
           <cell r="A163">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="164">
@@ -1044,7 +1192,7 @@
         </row>
         <row r="165">
           <cell r="A165">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="166">
@@ -1054,7 +1202,7 @@
         </row>
         <row r="167">
           <cell r="A167">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="168">
@@ -1069,7 +1217,7 @@
         </row>
         <row r="170">
           <cell r="A170">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="171">
@@ -1079,22 +1227,22 @@
         </row>
         <row r="172">
           <cell r="A172">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="173">
           <cell r="A173">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="174">
           <cell r="A174">
-            <v>13</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="175">
           <cell r="A175">
-            <v>16</v>
+            <v>13</v>
           </cell>
         </row>
         <row r="176">
@@ -1104,12 +1252,12 @@
         </row>
         <row r="177">
           <cell r="A177">
-            <v>0</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="178">
           <cell r="A178">
-            <v>12</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="179">
@@ -1124,7 +1272,7 @@
         </row>
         <row r="181">
           <cell r="A181">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="182">
@@ -1134,7 +1282,7 @@
         </row>
         <row r="183">
           <cell r="A183">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="184">
@@ -1149,7 +1297,7 @@
         </row>
         <row r="186">
           <cell r="A186">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="187">
@@ -1159,12 +1307,12 @@
         </row>
         <row r="188">
           <cell r="A188">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="189">
           <cell r="A189">
-            <v>0</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="190">
@@ -1174,17 +1322,17 @@
         </row>
         <row r="191">
           <cell r="A191">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="192">
           <cell r="A192">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="193">
           <cell r="A193">
-            <v>12</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="194">
@@ -1194,32 +1342,32 @@
         </row>
         <row r="195">
           <cell r="A195">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="196">
           <cell r="A196">
-            <v>0</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="197">
           <cell r="A197">
-            <v>2</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="198">
           <cell r="A198">
-            <v>10</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="199">
           <cell r="A199">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="200">
           <cell r="A200">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="201">
@@ -1229,7 +1377,7 @@
         </row>
         <row r="202">
           <cell r="A202">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="203">
@@ -1249,27 +1397,27 @@
         </row>
         <row r="206">
           <cell r="A206">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="207">
           <cell r="A207">
-            <v>2</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="208">
           <cell r="A208">
-            <v>10</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="209">
           <cell r="A209">
-            <v>2</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="210">
           <cell r="A210">
-            <v>10</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="211">
@@ -1299,17 +1447,17 @@
         </row>
         <row r="216">
           <cell r="A216">
-            <v>2</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="217">
           <cell r="A217">
-            <v>0</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="218">
           <cell r="A218">
-            <v>2</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="219">
@@ -1319,7 +1467,7 @@
         </row>
         <row r="220">
           <cell r="A220">
-            <v>1</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="221">
@@ -1329,12 +1477,12 @@
         </row>
         <row r="222">
           <cell r="A222">
-            <v>2</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="223">
           <cell r="A223">
-            <v>10</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="224">
@@ -1349,12 +1497,12 @@
         </row>
         <row r="226">
           <cell r="A226">
-            <v>2</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="227">
           <cell r="A227">
-            <v>10</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="228">
@@ -1374,12 +1522,12 @@
         </row>
         <row r="231">
           <cell r="A231">
-            <v>2</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="232">
           <cell r="A232">
-            <v>1</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="233">
@@ -1389,22 +1537,22 @@
         </row>
         <row r="234">
           <cell r="A234">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="235">
           <cell r="A235">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="236">
           <cell r="A236">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="237">
           <cell r="A237">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="238">
@@ -1424,17 +1572,17 @@
         </row>
         <row r="241">
           <cell r="A241">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="242">
           <cell r="A242">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="243">
           <cell r="A243">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="244">
@@ -1444,27 +1592,27 @@
         </row>
         <row r="245">
           <cell r="A245">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="246">
           <cell r="A246">
-            <v>5</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="247">
           <cell r="A247">
-            <v>10</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="248">
           <cell r="A248">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="249">
           <cell r="A249">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="250">
@@ -1474,7 +1622,7 @@
         </row>
         <row r="251">
           <cell r="A251">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="252">
@@ -1494,22 +1642,22 @@
         </row>
         <row r="255">
           <cell r="A255">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="256">
           <cell r="A256">
-            <v>6</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="257">
           <cell r="A257">
-            <v>12</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="258">
           <cell r="A258">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="259">
@@ -1524,7 +1672,7 @@
         </row>
         <row r="261">
           <cell r="A261">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="262">
@@ -1554,12 +1702,12 @@
         </row>
         <row r="267">
           <cell r="A267">
-            <v>6</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="268">
           <cell r="A268">
-            <v>10</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="269">
@@ -1624,17 +1772,17 @@
         </row>
         <row r="281">
           <cell r="A281">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="282">
           <cell r="A282">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="283">
           <cell r="A283">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="284">
@@ -1674,7 +1822,7 @@
         </row>
         <row r="291">
           <cell r="A291">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="292">
@@ -1699,7 +1847,7 @@
         </row>
         <row r="296">
           <cell r="A296">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="297">
@@ -1714,7 +1862,7 @@
         </row>
         <row r="299">
           <cell r="A299">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="300">
@@ -1829,12 +1977,12 @@
         </row>
         <row r="322">
           <cell r="A322">
-            <v>13</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="323">
           <cell r="A323">
-            <v>12</v>
+            <v>13</v>
           </cell>
         </row>
         <row r="324">
@@ -1849,7 +1997,7 @@
         </row>
         <row r="326">
           <cell r="A326">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="327">
@@ -1864,7 +2012,7 @@
         </row>
         <row r="329">
           <cell r="A329">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="330">
@@ -2279,12 +2427,12 @@
         </row>
         <row r="412">
           <cell r="A412">
-            <v>0</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="413">
           <cell r="A413">
-            <v>12</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="414">
@@ -2334,7 +2482,7 @@
         </row>
         <row r="423">
           <cell r="A423">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="424">
@@ -2354,7 +2502,7 @@
         </row>
         <row r="427">
           <cell r="A427">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="428">
@@ -2419,7 +2567,7 @@
         </row>
         <row r="440">
           <cell r="A440">
-            <v>0</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="441">
@@ -2429,12 +2577,12 @@
         </row>
         <row r="442">
           <cell r="A442">
-            <v>10</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="443">
           <cell r="A443">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="444">
@@ -2649,12 +2797,12 @@
         </row>
         <row r="486">
           <cell r="A486">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="487">
           <cell r="A487">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="488">
@@ -2669,7 +2817,7 @@
         </row>
         <row r="490">
           <cell r="A490">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="491">
@@ -2754,7 +2902,7 @@
         </row>
         <row r="507">
           <cell r="A507">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="508">
@@ -2794,7 +2942,7 @@
         </row>
         <row r="515">
           <cell r="A515">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="516">
@@ -2814,12 +2962,12 @@
         </row>
         <row r="519">
           <cell r="A519">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="520">
           <cell r="A520">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="521">
@@ -2834,7 +2982,7 @@
         </row>
         <row r="523">
           <cell r="A523">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="524">
@@ -2854,17 +3002,17 @@
         </row>
         <row r="527">
           <cell r="A527">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="528">
           <cell r="A528">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="529">
           <cell r="A529">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="530">
@@ -2874,7 +3022,7 @@
         </row>
         <row r="531">
           <cell r="A531">
-            <v>13</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="532">
@@ -2889,7 +3037,7 @@
         </row>
         <row r="534">
           <cell r="A534">
-            <v>12</v>
+            <v>13</v>
           </cell>
         </row>
         <row r="535">
@@ -2919,7 +3067,7 @@
         </row>
         <row r="540">
           <cell r="A540">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="541">
@@ -2934,32 +3082,32 @@
         </row>
         <row r="543">
           <cell r="A543">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="544">
           <cell r="A544">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="545">
           <cell r="A545">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="546">
           <cell r="A546">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="547">
           <cell r="A547">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="548">
           <cell r="A548">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="549">
@@ -2969,7 +3117,7 @@
         </row>
         <row r="550">
           <cell r="A550">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="551">
@@ -2979,17 +3127,17 @@
         </row>
         <row r="552">
           <cell r="A552">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="553">
           <cell r="A553">
-            <v>0</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="554">
           <cell r="A554">
-            <v>12</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="555">
@@ -2999,7 +3147,7 @@
         </row>
         <row r="556">
           <cell r="A556">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="557">
@@ -3009,7 +3157,7 @@
         </row>
         <row r="558">
           <cell r="A558">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="559">
@@ -3019,12 +3167,12 @@
         </row>
         <row r="560">
           <cell r="A560">
-            <v>5</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="561">
           <cell r="A561">
-            <v>1</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="562">
@@ -3074,7 +3222,7 @@
         </row>
         <row r="571">
           <cell r="A571">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="572">
@@ -3094,12 +3242,12 @@
         </row>
         <row r="575">
           <cell r="A575">
-            <v>5</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="576">
           <cell r="A576">
-            <v>10</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="577">
@@ -3119,7 +3267,7 @@
         </row>
         <row r="580">
           <cell r="A580">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="581">
@@ -3129,7 +3277,7 @@
         </row>
         <row r="582">
           <cell r="A582">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="583">
@@ -3149,22 +3297,22 @@
         </row>
         <row r="586">
           <cell r="A586">
-            <v>9</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="587">
           <cell r="A587">
-            <v>10</v>
+            <v>9</v>
           </cell>
         </row>
         <row r="588">
           <cell r="A588">
-            <v>9</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="589">
           <cell r="A589">
-            <v>1</v>
+            <v>9</v>
           </cell>
         </row>
         <row r="590">
@@ -3194,7 +3342,7 @@
         </row>
         <row r="595">
           <cell r="A595">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="596">
@@ -3274,22 +3422,22 @@
         </row>
         <row r="611">
           <cell r="A611">
-            <v>9</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="612">
           <cell r="A612">
-            <v>10</v>
+            <v>9</v>
           </cell>
         </row>
         <row r="613">
           <cell r="A613">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="614">
           <cell r="A614">
-            <v>16</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="615">
@@ -3319,7 +3467,7 @@
         </row>
         <row r="620">
           <cell r="A620">
-            <v>12</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="621">
@@ -3339,7 +3487,7 @@
         </row>
         <row r="624">
           <cell r="A624">
-            <v>16</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="625">
@@ -3359,32 +3507,32 @@
         </row>
         <row r="628">
           <cell r="A628">
-            <v>13</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="629">
           <cell r="A629">
-            <v>12</v>
+            <v>13</v>
           </cell>
         </row>
         <row r="630">
           <cell r="A630">
-            <v>5</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="631">
           <cell r="A631">
-            <v>1</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="632">
           <cell r="A632">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="633">
           <cell r="A633">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="634">
@@ -3404,12 +3552,12 @@
         </row>
         <row r="637">
           <cell r="A637">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="638">
           <cell r="A638">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="639">
@@ -3434,22 +3582,22 @@
         </row>
         <row r="643">
           <cell r="A643">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="644">
           <cell r="A644">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="645">
           <cell r="A645">
-            <v>5</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="646">
           <cell r="A646">
-            <v>12</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="647">
@@ -3459,7 +3607,7 @@
         </row>
         <row r="648">
           <cell r="A648">
-            <v>16</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="649">
@@ -3469,12 +3617,12 @@
         </row>
         <row r="650">
           <cell r="A650">
-            <v>14</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="651">
           <cell r="A651">
-            <v>16</v>
+            <v>14</v>
           </cell>
         </row>
         <row r="652">
@@ -3499,7 +3647,7 @@
         </row>
         <row r="656">
           <cell r="A656">
-            <v>12</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="657">
@@ -3509,7 +3657,7 @@
         </row>
         <row r="658">
           <cell r="A658">
-            <v>16</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="659">
@@ -3529,12 +3677,12 @@
         </row>
         <row r="662">
           <cell r="A662">
-            <v>1</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="663">
           <cell r="A663">
-            <v>16</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="664">
@@ -3629,12 +3777,12 @@
         </row>
         <row r="682">
           <cell r="A682">
-            <v>14</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="683">
           <cell r="A683">
-            <v>16</v>
+            <v>14</v>
           </cell>
         </row>
         <row r="684">
@@ -3649,7 +3797,7 @@
         </row>
         <row r="686">
           <cell r="A686">
-            <v>12</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="687">
@@ -3674,12 +3822,12 @@
         </row>
         <row r="691">
           <cell r="A691">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="692">
           <cell r="A692">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="693">
@@ -3744,7 +3892,7 @@
         </row>
         <row r="705">
           <cell r="A705">
-            <v>15</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="706">
@@ -3754,7 +3902,7 @@
         </row>
         <row r="707">
           <cell r="A707">
-            <v>12</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="708">
@@ -3794,12 +3942,12 @@
         </row>
         <row r="715">
           <cell r="A715">
-            <v>15</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="716">
           <cell r="A716">
-            <v>10</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="717">
@@ -3809,22 +3957,22 @@
         </row>
         <row r="718">
           <cell r="A718">
-            <v>0</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="719">
           <cell r="A719">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="720">
           <cell r="A720">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="721">
           <cell r="A721">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="722">
@@ -3839,7 +3987,7 @@
         </row>
         <row r="724">
           <cell r="A724">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="725">
@@ -3864,12 +4012,12 @@
         </row>
         <row r="729">
           <cell r="A729">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="730">
           <cell r="A730">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="731">
@@ -3879,17 +4027,17 @@
         </row>
         <row r="732">
           <cell r="A732">
-            <v>0</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="733">
           <cell r="A733">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="734">
           <cell r="A734">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="735">
@@ -3904,12 +4052,12 @@
         </row>
         <row r="737">
           <cell r="A737">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="738">
           <cell r="A738">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="739">
@@ -3949,7 +4097,7 @@
         </row>
         <row r="746">
           <cell r="A746">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="747">
@@ -3959,7 +4107,7 @@
         </row>
         <row r="748">
           <cell r="A748">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="749">
@@ -3999,32 +4147,32 @@
         </row>
         <row r="756">
           <cell r="A756">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="757">
           <cell r="A757">
-            <v>3</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="758">
           <cell r="A758">
-            <v>1</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="759">
           <cell r="A759">
-            <v>3</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="760">
           <cell r="A760">
-            <v>1</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="761">
           <cell r="A761">
-            <v>3</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="762">
@@ -4049,7 +4197,7 @@
         </row>
         <row r="766">
           <cell r="A766">
-            <v>12</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="767">
@@ -4139,12 +4287,12 @@
         </row>
         <row r="784">
           <cell r="A784">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="785">
           <cell r="A785">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="786">
@@ -4174,7 +4322,7 @@
         </row>
         <row r="791">
           <cell r="A791">
-            <v>3</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="792">
@@ -4189,7 +4337,7 @@
         </row>
         <row r="794">
           <cell r="A794">
-            <v>1</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="795">
@@ -4199,7 +4347,7 @@
         </row>
         <row r="796">
           <cell r="A796">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="797">
@@ -4219,7 +4367,7 @@
         </row>
         <row r="800">
           <cell r="A800">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="801">
@@ -4274,7 +4422,7 @@
         </row>
         <row r="811">
           <cell r="A811">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="812">
@@ -4289,12 +4437,12 @@
         </row>
         <row r="814">
           <cell r="A814">
-            <v>0</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="815">
           <cell r="A815">
-            <v>10</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="816">
@@ -4309,17 +4457,17 @@
         </row>
         <row r="818">
           <cell r="A818">
-            <v>0</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="819">
           <cell r="A819">
-            <v>12</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="820">
           <cell r="A820">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="821">
@@ -4329,7 +4477,7 @@
         </row>
         <row r="822">
           <cell r="A822">
-            <v>3</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="823">
@@ -4349,7 +4497,7 @@
         </row>
         <row r="826">
           <cell r="A826">
-            <v>12</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="827">
@@ -4444,12 +4592,12 @@
         </row>
         <row r="845">
           <cell r="A845">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="846">
           <cell r="A846">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="847">
@@ -4494,7 +4642,7 @@
         </row>
         <row r="855">
           <cell r="A855">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="856">
@@ -4509,7 +4657,7 @@
         </row>
         <row r="858">
           <cell r="A858">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="859">
@@ -4564,12 +4712,12 @@
         </row>
         <row r="869">
           <cell r="A869">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="870">
           <cell r="A870">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="871">
@@ -4619,7 +4767,7 @@
         </row>
         <row r="880">
           <cell r="A880">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="881">
@@ -4634,7 +4782,7 @@
         </row>
         <row r="883">
           <cell r="A883">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="884">
@@ -4649,7 +4797,7 @@
         </row>
         <row r="886">
           <cell r="A886">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="887">
@@ -4669,7 +4817,7 @@
         </row>
         <row r="890">
           <cell r="A890">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="891">
@@ -4684,7 +4832,7 @@
         </row>
         <row r="893">
           <cell r="A893">
-            <v>3</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="894">
@@ -4694,7 +4842,7 @@
         </row>
         <row r="895">
           <cell r="A895">
-            <v>12</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="896">
@@ -4719,7 +4867,7 @@
         </row>
         <row r="900">
           <cell r="A900">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="901">
@@ -4734,7 +4882,7 @@
         </row>
         <row r="903">
           <cell r="A903">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="904">
@@ -4759,7 +4907,7 @@
         </row>
         <row r="908">
           <cell r="A908">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="909">
@@ -4779,22 +4927,22 @@
         </row>
         <row r="912">
           <cell r="A912">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="913">
           <cell r="A913">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="914">
           <cell r="A914">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="915">
           <cell r="A915">
-            <v>3</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="916">
@@ -4804,7 +4952,7 @@
         </row>
         <row r="917">
           <cell r="A917">
-            <v>12</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="918">
@@ -4869,12 +5017,12 @@
         </row>
         <row r="930">
           <cell r="A930">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="931">
           <cell r="A931">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="932">
@@ -4884,7 +5032,7 @@
         </row>
         <row r="933">
           <cell r="A933">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="934">
@@ -4899,7 +5047,7 @@
         </row>
         <row r="936">
           <cell r="A936">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="937">
@@ -4919,17 +5067,17 @@
         </row>
         <row r="940">
           <cell r="A940">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="941">
           <cell r="A941">
-            <v>5</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="942">
           <cell r="A942">
-            <v>1</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="943">
@@ -4939,7 +5087,7 @@
         </row>
         <row r="944">
           <cell r="A944">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="945">
@@ -4949,12 +5097,12 @@
         </row>
         <row r="946">
           <cell r="A946">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="947">
           <cell r="A947">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="948">
@@ -5119,7 +5267,7 @@
         </row>
         <row r="980">
           <cell r="A980">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="981">
@@ -5129,12 +5277,12 @@
         </row>
         <row r="982">
           <cell r="A982">
-            <v>13</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="983">
           <cell r="A983">
-            <v>12</v>
+            <v>13</v>
           </cell>
         </row>
         <row r="984">
@@ -5149,7 +5297,7 @@
         </row>
         <row r="986">
           <cell r="A986">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="987">
@@ -5164,12 +5312,12 @@
         </row>
         <row r="989">
           <cell r="A989">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="990">
           <cell r="A990">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="991">
@@ -5284,12 +5432,12 @@
         </row>
         <row r="1013">
           <cell r="A1013">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1014">
           <cell r="A1014">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1015">
@@ -5494,12 +5642,12 @@
         </row>
         <row r="1055">
           <cell r="A1055">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1056">
           <cell r="A1056">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1057">
@@ -5544,7 +5692,7 @@
         </row>
         <row r="1065">
           <cell r="A1065">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1066">
@@ -5609,7 +5757,7 @@
         </row>
         <row r="1078">
           <cell r="A1078">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1079">
@@ -5674,12 +5822,12 @@
         </row>
         <row r="1091">
           <cell r="A1091">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1092">
           <cell r="A1092">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1093">
@@ -5689,12 +5837,12 @@
         </row>
         <row r="1094">
           <cell r="A1094">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1095">
           <cell r="A1095">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1096">
@@ -5894,12 +6042,12 @@
         </row>
         <row r="1135">
           <cell r="A1135">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1136">
           <cell r="A1136">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1137">
@@ -5909,7 +6057,7 @@
         </row>
         <row r="1138">
           <cell r="A1138">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1139">
@@ -5929,7 +6077,7 @@
         </row>
         <row r="1142">
           <cell r="A1142">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1143">
@@ -6064,12 +6212,12 @@
         </row>
         <row r="1169">
           <cell r="A1169">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1170">
           <cell r="A1170">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1171">
@@ -6084,12 +6232,12 @@
         </row>
         <row r="1173">
           <cell r="A1173">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1174">
           <cell r="A1174">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1175">
@@ -6169,7 +6317,7 @@
         </row>
         <row r="1190">
           <cell r="A1190">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1191">
@@ -6349,12 +6497,12 @@
         </row>
         <row r="1226">
           <cell r="A1226">
-            <v>8</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1227">
           <cell r="A1227">
-            <v>10</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="1228">
@@ -6364,7 +6512,7 @@
         </row>
         <row r="1229">
           <cell r="A1229">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1230">
@@ -6844,12 +6992,12 @@
         </row>
         <row r="1325">
           <cell r="A1325">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1326">
           <cell r="A1326">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1327">
@@ -6864,12 +7012,12 @@
         </row>
         <row r="1329">
           <cell r="A1329">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1330">
           <cell r="A1330">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1331">
@@ -6879,12 +7027,12 @@
         </row>
         <row r="1332">
           <cell r="A1332">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1333">
           <cell r="A1333">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1334">
@@ -6899,7 +7047,7 @@
         </row>
         <row r="1336">
           <cell r="A1336">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1337">
@@ -6909,12 +7057,12 @@
         </row>
         <row r="1338">
           <cell r="A1338">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1339">
           <cell r="A1339">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1340">
@@ -6939,7 +7087,7 @@
         </row>
         <row r="1344">
           <cell r="A1344">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1345">
@@ -6969,7 +7117,7 @@
         </row>
         <row r="1350">
           <cell r="A1350">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1351">
@@ -7014,12 +7162,12 @@
         </row>
         <row r="1359">
           <cell r="A1359">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1360">
           <cell r="A1360">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1361">
@@ -7039,17 +7187,17 @@
         </row>
         <row r="1364">
           <cell r="A1364">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1365">
           <cell r="A1365">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1366">
           <cell r="A1366">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1367">
@@ -7089,7 +7237,7 @@
         </row>
         <row r="1374">
           <cell r="A1374">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1375">
@@ -7114,7 +7262,7 @@
         </row>
         <row r="1379">
           <cell r="A1379">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1380">
@@ -7129,7 +7277,7 @@
         </row>
         <row r="1382">
           <cell r="A1382">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1383">
@@ -7159,7 +7307,7 @@
         </row>
         <row r="1388">
           <cell r="A1388">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1389">
@@ -7199,7 +7347,7 @@
         </row>
         <row r="1396">
           <cell r="A1396">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1397">
@@ -7219,7 +7367,7 @@
         </row>
         <row r="1400">
           <cell r="A1400">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1401">
@@ -7299,7 +7447,7 @@
         </row>
         <row r="1416">
           <cell r="A1416">
-            <v>16</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1417">
@@ -7319,22 +7467,22 @@
         </row>
         <row r="1420">
           <cell r="A1420">
-            <v>5</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="1421">
           <cell r="A1421">
-            <v>9</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="1422">
           <cell r="A1422">
-            <v>10</v>
+            <v>9</v>
           </cell>
         </row>
         <row r="1423">
           <cell r="A1423">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1424">
@@ -7359,12 +7507,12 @@
         </row>
         <row r="1428">
           <cell r="A1428">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1429">
           <cell r="A1429">
-            <v>12</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="1430">
@@ -7444,7 +7592,7 @@
         </row>
         <row r="1445">
           <cell r="A1445">
-            <v>16</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1446">
@@ -7464,32 +7612,32 @@
         </row>
         <row r="1449">
           <cell r="A1449">
-            <v>5</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="1450">
           <cell r="A1450">
-            <v>9</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="1451">
           <cell r="A1451">
-            <v>10</v>
+            <v>9</v>
           </cell>
         </row>
         <row r="1452">
           <cell r="A1452">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1453">
           <cell r="A1453">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1454">
           <cell r="A1454">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1455">
@@ -7499,7 +7647,7 @@
         </row>
         <row r="1456">
           <cell r="A1456">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1457">
@@ -7509,12 +7657,12 @@
         </row>
         <row r="1458">
           <cell r="A1458">
-            <v>0</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1459">
           <cell r="A1459">
-            <v>10</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="1460">
@@ -7524,22 +7672,22 @@
         </row>
         <row r="1461">
           <cell r="A1461">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1462">
           <cell r="A1462">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1463">
           <cell r="A1463">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1464">
           <cell r="A1464">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1465">
@@ -7549,12 +7697,12 @@
         </row>
         <row r="1466">
           <cell r="A1466">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1467">
           <cell r="A1467">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1468">
@@ -7569,32 +7717,32 @@
         </row>
         <row r="1470">
           <cell r="A1470">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1471">
           <cell r="A1471">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1472">
           <cell r="A1472">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1473">
           <cell r="A1473">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1474">
           <cell r="A1474">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1475">
           <cell r="A1475">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1476">
@@ -7604,42 +7752,42 @@
         </row>
         <row r="1477">
           <cell r="A1477">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1478">
           <cell r="A1478">
-            <v>16</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1479">
           <cell r="A1479">
-            <v>1</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="1480">
           <cell r="A1480">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1481">
           <cell r="A1481">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1482">
           <cell r="A1482">
-            <v>0</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1483">
           <cell r="A1483">
-            <v>12</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="1484">
           <cell r="A1484">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1485">
@@ -7654,12 +7802,12 @@
         </row>
         <row r="1487">
           <cell r="A1487">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1488">
           <cell r="A1488">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1489">
@@ -7669,22 +7817,22 @@
         </row>
         <row r="1490">
           <cell r="A1490">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1491">
           <cell r="A1491">
-            <v>0</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1492">
           <cell r="A1492">
-            <v>5</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="1493">
           <cell r="A1493">
-            <v>6</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="1494">
@@ -7694,12 +7842,12 @@
         </row>
         <row r="1495">
           <cell r="A1495">
-            <v>5</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="1496">
           <cell r="A1496">
-            <v>1</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="1497">
@@ -7739,7 +7887,7 @@
         </row>
         <row r="1504">
           <cell r="A1504">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1505">
@@ -7759,7 +7907,7 @@
         </row>
         <row r="1508">
           <cell r="A1508">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1509">
@@ -7769,7 +7917,7 @@
         </row>
         <row r="1510">
           <cell r="A1510">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1511">
@@ -7789,7 +7937,7 @@
         </row>
         <row r="1514">
           <cell r="A1514">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1515">
@@ -7799,7 +7947,7 @@
         </row>
         <row r="1516">
           <cell r="A1516">
-            <v>16</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1517">
@@ -7829,7 +7977,7 @@
         </row>
         <row r="1522">
           <cell r="A1522">
-            <v>12</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="1523">
@@ -7849,7 +7997,7 @@
         </row>
         <row r="1526">
           <cell r="A1526">
-            <v>16</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1527">
@@ -7869,22 +8017,22 @@
         </row>
         <row r="1530">
           <cell r="A1530">
-            <v>12</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="1531">
           <cell r="A1531">
-            <v>5</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1532">
           <cell r="A1532">
-            <v>1</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="1533">
           <cell r="A1533">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1534">
@@ -7899,7 +8047,7 @@
         </row>
         <row r="1536">
           <cell r="A1536">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1537">
@@ -7924,12 +8072,12 @@
         </row>
         <row r="1541">
           <cell r="A1541">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1542">
           <cell r="A1542">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1543">
@@ -7959,17 +8107,17 @@
         </row>
         <row r="1548">
           <cell r="A1548">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1549">
           <cell r="A1549">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1550">
           <cell r="A1550">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1551">
@@ -7979,7 +8127,7 @@
         </row>
         <row r="1552">
           <cell r="A1552">
-            <v>16</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1553">
@@ -7989,12 +8137,12 @@
         </row>
         <row r="1554">
           <cell r="A1554">
-            <v>14</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="1555">
           <cell r="A1555">
-            <v>16</v>
+            <v>14</v>
           </cell>
         </row>
         <row r="1556">
@@ -8019,7 +8167,7 @@
         </row>
         <row r="1560">
           <cell r="A1560">
-            <v>12</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="1561">
@@ -8029,7 +8177,7 @@
         </row>
         <row r="1562">
           <cell r="A1562">
-            <v>16</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1563">
@@ -8049,12 +8197,12 @@
         </row>
         <row r="1566">
           <cell r="A1566">
-            <v>1</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="1567">
           <cell r="A1567">
-            <v>16</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1568">
@@ -8149,12 +8297,12 @@
         </row>
         <row r="1586">
           <cell r="A1586">
-            <v>14</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="1587">
           <cell r="A1587">
-            <v>16</v>
+            <v>14</v>
           </cell>
         </row>
         <row r="1588">
@@ -8169,7 +8317,7 @@
         </row>
         <row r="1590">
           <cell r="A1590">
-            <v>10</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="1591">
@@ -8199,7 +8347,7 @@
         </row>
         <row r="1596">
           <cell r="A1596">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1597">
@@ -8209,7 +8357,7 @@
         </row>
         <row r="1598">
           <cell r="A1598">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1599">
@@ -8219,7 +8367,7 @@
         </row>
         <row r="1600">
           <cell r="A1600">
-            <v>0</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1601">
@@ -8229,7 +8377,7 @@
         </row>
         <row r="1602">
           <cell r="A1602">
-            <v>10</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="1603">
@@ -8249,7 +8397,7 @@
         </row>
         <row r="1606">
           <cell r="A1606">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1607">
@@ -8274,12 +8422,12 @@
         </row>
         <row r="1611">
           <cell r="A1611">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1612">
           <cell r="A1612">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1613">
@@ -8299,12 +8447,12 @@
         </row>
         <row r="1616">
           <cell r="A1616">
-            <v>15</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1617">
           <cell r="A1617">
-            <v>12</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="1618">
@@ -8349,12 +8497,12 @@
         </row>
         <row r="1626">
           <cell r="A1626">
-            <v>15</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1627">
           <cell r="A1627">
-            <v>12</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="1628">
@@ -8394,32 +8542,32 @@
         </row>
         <row r="1635">
           <cell r="A1635">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1636">
           <cell r="A1636">
-            <v>3</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1637">
           <cell r="A1637">
-            <v>1</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="1638">
           <cell r="A1638">
-            <v>3</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1639">
           <cell r="A1639">
-            <v>1</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="1640">
           <cell r="A1640">
-            <v>3</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1641">
@@ -8444,7 +8592,7 @@
         </row>
         <row r="1645">
           <cell r="A1645">
-            <v>12</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="1646">
@@ -8724,7 +8872,7 @@
         </row>
         <row r="1701">
           <cell r="A1701">
-            <v>3</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1702">
@@ -8739,7 +8887,7 @@
         </row>
         <row r="1704">
           <cell r="A1704">
-            <v>1</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="1705">
@@ -8759,7 +8907,7 @@
         </row>
         <row r="1708">
           <cell r="A1708">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1709">
@@ -8779,12 +8927,12 @@
         </row>
         <row r="1712">
           <cell r="A1712">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1713">
           <cell r="A1713">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1714">
@@ -8794,17 +8942,17 @@
         </row>
         <row r="1715">
           <cell r="A1715">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1716">
           <cell r="A1716">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1717">
           <cell r="A1717">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1718">
@@ -8819,7 +8967,7 @@
         </row>
         <row r="1720">
           <cell r="A1720">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1721">
@@ -8834,7 +8982,7 @@
         </row>
         <row r="1723">
           <cell r="A1723">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1724">
@@ -8909,7 +9057,7 @@
         </row>
         <row r="1738">
           <cell r="A1738">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1739">
@@ -8924,27 +9072,27 @@
         </row>
         <row r="1741">
           <cell r="A1741">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1742">
           <cell r="A1742">
-            <v>12</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="1743">
           <cell r="A1743">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1744">
           <cell r="A1744">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1745">
           <cell r="A1745">
-            <v>1</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1746">
@@ -8954,7 +9102,7 @@
         </row>
         <row r="1747">
           <cell r="A1747">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1748">
@@ -8964,7 +9112,7 @@
         </row>
         <row r="1749">
           <cell r="A1749">
-            <v>3</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1750">
@@ -8984,7 +9132,7 @@
         </row>
         <row r="1753">
           <cell r="A1753">
-            <v>12</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="1754">
@@ -9084,12 +9232,12 @@
         </row>
         <row r="1773">
           <cell r="A1773">
-            <v>15</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1774">
           <cell r="A1774">
-            <v>12</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="1775">
@@ -9139,7 +9287,7 @@
         </row>
         <row r="1784">
           <cell r="A1784">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1785">
@@ -9154,7 +9302,7 @@
         </row>
         <row r="1787">
           <cell r="A1787">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1788">
@@ -9164,7 +9312,7 @@
         </row>
         <row r="1789">
           <cell r="A1789">
-            <v>12</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="1790">
@@ -9304,17 +9452,17 @@
         </row>
         <row r="1817">
           <cell r="A1817">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1818">
           <cell r="A1818">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1819">
           <cell r="A1819">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1820">
@@ -9329,7 +9477,7 @@
         </row>
         <row r="1822">
           <cell r="A1822">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1823">
@@ -9344,7 +9492,7 @@
         </row>
         <row r="1825">
           <cell r="A1825">
-            <v>3</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1826">
@@ -9354,7 +9502,7 @@
         </row>
         <row r="1827">
           <cell r="A1827">
-            <v>12</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="1828">
@@ -9404,7 +9552,7 @@
         </row>
         <row r="1837">
           <cell r="A1837">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1838">
@@ -9414,7 +9562,7 @@
         </row>
         <row r="1839">
           <cell r="A1839">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1840">
@@ -9444,7 +9592,7 @@
         </row>
         <row r="1845">
           <cell r="A1845">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1846">
@@ -9459,17 +9607,17 @@
         </row>
         <row r="1848">
           <cell r="A1848">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1849">
           <cell r="A1849">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1850">
           <cell r="A1850">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1851">
@@ -9524,12 +9672,12 @@
         </row>
         <row r="1861">
           <cell r="A1861">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1862">
           <cell r="A1862">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1863">
@@ -9539,7 +9687,7 @@
         </row>
         <row r="1864">
           <cell r="A1864">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1865">
@@ -9564,17 +9712,17 @@
         </row>
         <row r="1869">
           <cell r="A1869">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1870">
           <cell r="A1870">
-            <v>12</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1871">
           <cell r="A1871">
-            <v>10</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="1872">
@@ -9584,17 +9732,17 @@
         </row>
         <row r="1873">
           <cell r="A1873">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="1874">
           <cell r="A1874">
-            <v>5</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="1875">
           <cell r="A1875">
-            <v>1</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="1876">
@@ -9905,15 +10053,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AF6FC4-0EAD-462F-8939-DE8EFB9F21E3}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:BJ27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
@@ -9931,7 +10079,7 @@
     <col min="17" max="17" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9941,8 +10089,11 @@
       <c r="C1" t="s">
         <v>18</v>
       </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -9953,8 +10104,17 @@
         <f>COUNTIF('[1]Data File'!$A$1:$A$1876,A2)</f>
         <v>38</v>
       </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -9963,10 +10123,19 @@
       </c>
       <c r="C3">
         <f>COUNTIF('[1]Data File'!$A$1:$A$1876,A3)</f>
-        <v>200</v>
+        <v>199</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -9977,8 +10146,35 @@
         <f>COUNTIF('[1]Data File'!$A$1:$A$1876,A4)</f>
         <v>11</v>
       </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>11</v>
+      </c>
+      <c r="M4">
+        <v>13</v>
+      </c>
+      <c r="N4">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -9989,8 +10185,26 @@
         <f>COUNTIF('[1]Data File'!$A$1:$A$1876,A5)</f>
         <v>34</v>
       </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>7</v>
+      </c>
+      <c r="K5">
+        <v>9</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -10001,8 +10215,26 @@
         <f>COUNTIF('[1]Data File'!$A$1:$A$1876,A6)</f>
         <v>4</v>
       </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>14</v>
+      </c>
+      <c r="K6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -10014,7 +10246,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -10026,7 +10258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -10038,7 +10270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -10050,7 +10282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -10062,7 +10294,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -10074,7 +10306,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -10086,7 +10318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -10098,7 +10330,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -10110,7 +10342,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -10122,7 +10354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -10134,7 +10366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -10146,13 +10378,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:62" x14ac:dyDescent="0.25">
       <c r="C22">
         <f>SUM(C2:C18)</f>
-        <v>1876</v>
+        <v>1875</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="1" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:62" s="1" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -10201,8 +10433,146 @@
       <c r="P26" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="Q26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AT26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AW26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AZ26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BA26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BB26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BE26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BF26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BH26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BI26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BJ26" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="27" spans="1:16" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:62" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>